<commit_message>
Removed Debug_workspace.mat on error.
</commit_message>
<xml_diff>
--- a/SupportingDocs/ICA_Prep_Values.xlsx
+++ b/SupportingDocs/ICA_Prep_Values.xlsx
@@ -13,7 +13,247 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
+  <si>
+    <t>SUBID</t>
+  </si>
+  <si>
+    <t>810</t>
+  </si>
+  <si>
+    <t>AmpthValue</t>
+  </si>
+  <si>
+    <t>WindowValue</t>
+  </si>
+  <si>
+    <t>StepValue</t>
+  </si>
+  <si>
+    <t>SUBID</t>
+  </si>
+  <si>
+    <t>810</t>
+  </si>
+  <si>
+    <t>AmpthValue</t>
+  </si>
+  <si>
+    <t>WindowValue</t>
+  </si>
+  <si>
+    <t>StepValue</t>
+  </si>
+  <si>
+    <t>SUBID</t>
+  </si>
+  <si>
+    <t>810</t>
+  </si>
+  <si>
+    <t>AmpthValue</t>
+  </si>
+  <si>
+    <t>WindowValue</t>
+  </si>
+  <si>
+    <t>StepValue</t>
+  </si>
+  <si>
+    <t>SUBID</t>
+  </si>
+  <si>
+    <t>810</t>
+  </si>
+  <si>
+    <t>AmpthValue</t>
+  </si>
+  <si>
+    <t>WindowValue</t>
+  </si>
+  <si>
+    <t>StepValue</t>
+  </si>
+  <si>
+    <t>SUBID</t>
+  </si>
+  <si>
+    <t>810</t>
+  </si>
+  <si>
+    <t>AmpthValue</t>
+  </si>
+  <si>
+    <t>WindowValue</t>
+  </si>
+  <si>
+    <t>StepValue</t>
+  </si>
+  <si>
+    <t>SUBID</t>
+  </si>
+  <si>
+    <t>810</t>
+  </si>
+  <si>
+    <t>AmpthValue</t>
+  </si>
+  <si>
+    <t>WindowValue</t>
+  </si>
+  <si>
+    <t>StepValue</t>
+  </si>
+  <si>
+    <t>SUBID</t>
+  </si>
+  <si>
+    <t>810</t>
+  </si>
+  <si>
+    <t>AmpthValue</t>
+  </si>
+  <si>
+    <t>WindowValue</t>
+  </si>
+  <si>
+    <t>StepValue</t>
+  </si>
+  <si>
+    <t>SUBID</t>
+  </si>
+  <si>
+    <t>810</t>
+  </si>
+  <si>
+    <t>AmpthValue</t>
+  </si>
+  <si>
+    <t>WindowValue</t>
+  </si>
+  <si>
+    <t>StepValue</t>
+  </si>
+  <si>
+    <t>SUBID</t>
+  </si>
+  <si>
+    <t>810</t>
+  </si>
+  <si>
+    <t>AmpthValue</t>
+  </si>
+  <si>
+    <t>WindowValue</t>
+  </si>
+  <si>
+    <t>StepValue</t>
+  </si>
+  <si>
+    <t>SUBID</t>
+  </si>
+  <si>
+    <t>810</t>
+  </si>
+  <si>
+    <t>AmpthValue</t>
+  </si>
+  <si>
+    <t>WindowValue</t>
+  </si>
+  <si>
+    <t>StepValue</t>
+  </si>
+  <si>
+    <t>SUBID</t>
+  </si>
+  <si>
+    <t>810</t>
+  </si>
+  <si>
+    <t>AmpthValue</t>
+  </si>
+  <si>
+    <t>WindowValue</t>
+  </si>
+  <si>
+    <t>StepValue</t>
+  </si>
+  <si>
+    <t>SUBID</t>
+  </si>
+  <si>
+    <t>810</t>
+  </si>
+  <si>
+    <t>AmpthValue</t>
+  </si>
+  <si>
+    <t>WindowValue</t>
+  </si>
+  <si>
+    <t>StepValue</t>
+  </si>
+  <si>
+    <t>SUBID</t>
+  </si>
+  <si>
+    <t>810</t>
+  </si>
+  <si>
+    <t>AmpthValue</t>
+  </si>
+  <si>
+    <t>WindowValue</t>
+  </si>
+  <si>
+    <t>StepValue</t>
+  </si>
+  <si>
+    <t>SUBID</t>
+  </si>
+  <si>
+    <t>810</t>
+  </si>
+  <si>
+    <t>AmpthValue</t>
+  </si>
+  <si>
+    <t>WindowValue</t>
+  </si>
+  <si>
+    <t>StepValue</t>
+  </si>
+  <si>
+    <t>SUBID</t>
+  </si>
+  <si>
+    <t>810</t>
+  </si>
+  <si>
+    <t>AmpthValue</t>
+  </si>
+  <si>
+    <t>WindowValue</t>
+  </si>
+  <si>
+    <t>StepValue</t>
+  </si>
+  <si>
+    <t>SUBID</t>
+  </si>
+  <si>
+    <t>810</t>
+  </si>
+  <si>
+    <t>AmpthValue</t>
+  </si>
+  <si>
+    <t>WindowValue</t>
+  </si>
+  <si>
+    <t>StepValue</t>
+  </si>
   <si>
     <t>SUBID</t>
   </si>
@@ -48,7 +288,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -57,13 +297,45 @@
       <diagonal/>
     </border>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -76,29 +348,29 @@
   <dimension ref="A1:D2"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" customWidth="true"/>
-    <col min="2" max="2" width="12.28515625" customWidth="true"/>
-    <col min="3" max="3" width="13.7109375" customWidth="true"/>
-    <col min="4" max="4" width="10.28515625" customWidth="true"/>
+    <col min="1" max="1" width="6.2578125" customWidth="true"/>
+    <col min="2" max="2" width="11.44140625" customWidth="true"/>
+    <col min="3" max="3" width="12.8046875" customWidth="true"/>
+    <col min="4" max="4" width="9.44140625" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>2</v>
+        <v>82</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>4</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>1</v>
+        <v>81</v>
       </c>
       <c r="B2" s="0">
         <v>500</v>

</xml_diff>